<commit_message>
Fixed tests due to alignment printing of annotated sequences.
</commit_message>
<xml_diff>
--- a/tests/data/segments.xlsx
+++ b/tests/data/segments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>PID</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>longTE</t>
+  </si>
+  <si>
+    <t>SPED KISQLKE KIQQLKQ ENQQLEE ENSQLEY ENQQLEE ENSQLEY</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +536,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>